<commit_message>
finalized comparison table for microcontroller
</commit_message>
<xml_diff>
--- a/Dokumentation/tables/BAT_Vergleich-Mikrocontroller.xlsx
+++ b/Dokumentation/tables/BAT_Vergleich-Mikrocontroller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Module\TA.BA_BAA+E.F2401\Entwicklung\Dokumentation\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A88822-10B3-4F68-976F-C47D22175BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2643611-6CD6-4B02-9B7C-F70085392B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="40">
   <si>
     <t>Hersteller</t>
   </si>
@@ -167,6 +167,15 @@
   <si>
     <t>ANT: NINA-B406-00B (u-blox)
           BL653 (Lairdconnect)</t>
+  </si>
+  <si>
+    <t>ANT: NORA-B106-00B (u-blox)
+          BL5340 (Lairdconnect)</t>
+  </si>
+  <si>
+    <t>ANT: NINA-B302-00B (u-blox)
+          BMD-340-A-R (u-blox)
+          BL654PA (Lairdconnect)</t>
   </si>
 </sst>
 </file>
@@ -565,7 +574,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +591,7 @@
     <col min="10" max="10" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -780,7 +789,9 @@
       <c r="J5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="L5" s="4">
         <v>58</v>
       </c>
@@ -819,7 +830,9 @@
       <c r="J6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4">
+        <v>512</v>
+      </c>
       <c r="L6" s="4">
         <v>52</v>
       </c>
@@ -827,7 +840,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -858,11 +871,15 @@
       <c r="J7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4">
+        <v>1024</v>
+      </c>
       <c r="L7" s="4">
         <v>52</v>
       </c>
-      <c r="M7" s="11"/>
+      <c r="M7" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -895,11 +912,15 @@
       <c r="J8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="4">
+        <v>1024</v>
+      </c>
       <c r="L8" s="4">
         <v>48</v>
       </c>
-      <c r="M8" s="11"/>
+      <c r="M8" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
@@ -979,7 +1000,9 @@
       <c r="L10" s="5">
         <v>29</v>
       </c>
-      <c r="M10" s="13"/>
+      <c r="M10" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
@@ -1055,7 +1078,9 @@
       <c r="L12" s="6">
         <v>18</v>
       </c>
-      <c r="M12" s="14"/>
+      <c r="M12" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M12">

</xml_diff>